<commit_message>
Re-test: now fully passes main testing program
</commit_message>
<xml_diff>
--- a/test/RefBasedMI testing summary.xlsx
+++ b/test/RefBasedMI testing summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\RefbasedMI\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FE8659-32B9-421E-AF66-16FCE5C2287E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2D0BF-20FD-442E-BE1F-D679654020FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="107">
   <si>
     <t>Ian main testing program.R</t>
   </si>
@@ -381,6 +381,13 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>0.0.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">works perfectly, and I checked that program output matches exactly
+</t>
   </si>
 </sst>
 </file>
@@ -507,7 +514,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -533,103 +540,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -652,25 +562,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -804,93 +695,137 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -910,25 +845,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -950,21 +866,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63A6B612-A08F-475A-B68C-2C6A25ECC80C}" name="Table1" displayName="Table1" ref="A2:L41" totalsRowShown="0" headerRowDxfId="25" dataDxfId="9" headerRowBorderDxfId="28" tableBorderDxfId="27">
-  <autoFilter ref="A2:L41" xr:uid="{63A6B612-A08F-475A-B68C-2C6A25ECC80C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63A6B612-A08F-475A-B68C-2C6A25ECC80C}" name="Table1" displayName="Table1" ref="A2:L43" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+  <autoFilter ref="A2:L43" xr:uid="{63A6B612-A08F-475A-B68C-2C6A25ECC80C}"/>
   <tableColumns count="12">
-    <tableColumn id="11" xr3:uid="{740CBD4F-CD6B-43BA-8C70-A1C50399F878}" name="Test" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{DE5F9776-A5F0-466E-8017-A561894C37CC}" name="Test program" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{F73C437D-1953-40F7-B786-65B34C033CAD}" name="Tester" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{216B41F4-96EB-4AE9-97C9-B7F4F96EA7F8}" name="Prog version" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{C8AFD595-D12A-43B3-8376-398EFA2E2631}" name="Prog date" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E66DE38B-E2AE-49D4-96B5-32E818D05F1A}" name="Date" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{BADA15A5-6183-4E6E-9682-948861E68C1C}" name="Passed?" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{1ABFFB10-4F59-4B59-BA12-19132EC5FB73}" name="Finding" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{79B75F80-A7D0-4341-888F-22C9B24CBDB2}" name="Note" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{20595CE3-0CEC-4D84-934E-FB4AC4782736}" name="Action" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{9C26D8EB-E269-4D7C-9FD6-ADC4F8D56709}" name="Note2" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{AB2661CC-C7DE-4471-99FD-CD761FADA6EF}" name="Live failure?" dataDxfId="10">
+    <tableColumn id="11" xr3:uid="{740CBD4F-CD6B-43BA-8C70-A1C50399F878}" name="Test" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{DE5F9776-A5F0-466E-8017-A561894C37CC}" name="Test program" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{F73C437D-1953-40F7-B786-65B34C033CAD}" name="Tester" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{216B41F4-96EB-4AE9-97C9-B7F4F96EA7F8}" name="Prog version" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{C8AFD595-D12A-43B3-8376-398EFA2E2631}" name="Prog date" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{E66DE38B-E2AE-49D4-96B5-32E818D05F1A}" name="Date" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{BADA15A5-6183-4E6E-9682-948861E68C1C}" name="Passed?" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1ABFFB10-4F59-4B59-BA12-19132EC5FB73}" name="Finding" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{79B75F80-A7D0-4341-888F-22C9B24CBDB2}" name="Note" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{20595CE3-0CEC-4D84-934E-FB4AC4782736}" name="Action" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{9C26D8EB-E269-4D7C-9FD6-ADC4F8D56709}" name="Note2" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{AB2661CC-C7DE-4471-99FD-CD761FADA6EF}" name="Live failure?" dataDxfId="4">
       <calculatedColumnFormula>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A4)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1277,13 +1193,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="I12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1389,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1950,47 +1866,35 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A20)))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="10">
-        <v>44494</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="10">
-        <v>44522</v>
+        <v>44749</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="J20" s="5"/>
-      <c r="K20" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="K20" s="5"/>
       <c r="L20" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A21)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="7" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>0</v>
@@ -2002,70 +1906,78 @@
         <v>95</v>
       </c>
       <c r="E21" s="10">
-        <v>44522</v>
+        <v>44494</v>
       </c>
       <c r="F21" s="10">
         <v>44522</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K21" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="L21" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A22)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="10"/>
+    <row r="22" spans="1:12" s="7" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="10">
+        <v>44522</v>
+      </c>
       <c r="F22" s="10">
-        <v>44698</v>
+        <v>44522</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A23)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="10">
-        <v>44719</v>
-      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="10">
-        <v>44726</v>
+        <v>44698</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -2075,199 +1987,195 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>14</v>
-      </c>
+    <row r="24" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" s="10">
-        <v>44522</v>
+        <v>44719</v>
       </c>
       <c r="F24" s="10">
-        <v>44680</v>
+        <v>44726</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="I24" s="5"/>
-      <c r="J24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
       <c r="L24" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A25)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="10"/>
+    <row r="25" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="10">
+        <v>44522</v>
+      </c>
       <c r="F25" s="10">
         <v>44680</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+      <c r="J25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="L25" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A26)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="10">
-        <v>44522</v>
-      </c>
+    <row r="26" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="10">
         <v>44680</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
       <c r="L26" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A27)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="10"/>
+    <row r="27" spans="1:12" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="10">
+        <v>44522</v>
+      </c>
       <c r="F27" s="10">
         <v>44680</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
+      <c r="J27" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="L27" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A28)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>97</v>
-      </c>
+    <row r="28" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10">
         <v>44680</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>76</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="K28" s="5"/>
       <c r="L28" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A29)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+    <row r="29" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10">
-        <v>44698</v>
+        <v>44680</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H29" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
+      <c r="K29" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="L29" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A30)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>97</v>
-      </c>
+    <row r="30" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10">
-        <v>44680</v>
+        <v>44698</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>78</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -2276,20 +2184,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+    <row r="31" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10">
-        <v>44698</v>
+        <v>44680</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -2303,63 +2219,63 @@
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="10">
-        <v>44719</v>
-      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="10">
-        <v>44726</v>
+        <v>44698</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H32" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="17" t="b">
+      <c r="L32" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A33)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>14</v>
-      </c>
+    <row r="33" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
       <c r="D33" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E33" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="E33" s="10">
+        <v>44719</v>
+      </c>
       <c r="F33" s="10">
-        <v>44680</v>
+        <v>44726</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>80</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="5" t="b">
+      <c r="L33" s="17" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A34)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+    <row r="34" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10">
         <v>44680</v>
@@ -2367,7 +2283,9 @@
       <c r="G34" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="5"/>
+      <c r="H34" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2380,17 +2298,13 @@
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" s="10">
-        <v>44719</v>
-      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="10"/>
       <c r="F35" s="10">
-        <v>44726</v>
+        <v>44680</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -2401,29 +2315,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>14</v>
-      </c>
+    <row r="36" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="E36" s="10">
+        <v>44719</v>
+      </c>
       <c r="F36" s="10">
-        <v>44680</v>
+        <v>44726</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>84</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -2432,22 +2340,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+    <row r="37" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10">
-        <v>44698</v>
+        <v>44680</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="H37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5" t="b">
@@ -2455,59 +2371,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E38" s="10">
-        <v>44719</v>
-      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="10"/>
       <c r="F38" s="10">
-        <v>44726</v>
+        <v>44698</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>102</v>
-      </c>
+      <c r="H38" s="5"/>
       <c r="I38" s="5" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A39)))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
       <c r="D39" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E39" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="E39" s="10">
+        <v>44719</v>
+      </c>
       <c r="F39" s="10">
-        <v>44698</v>
+        <v>44726</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I39" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5" t="b">
@@ -2515,23 +2423,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="E40" s="10">
-        <v>44719</v>
+        <v>44748</v>
       </c>
       <c r="F40" s="10">
-        <v>44726</v>
+        <v>44749</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H40" s="5"/>
+      <c r="H40" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -2540,35 +2450,101 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="5"/>
+      <c r="F41" s="10">
+        <v>44698</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="17" t="b">
+      <c r="L41" s="5" t="b">
         <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A42)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="10">
+        <v>44719</v>
+      </c>
+      <c r="F42" s="10">
+        <v>44726</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5" t="b">
+        <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A43)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="17" t="b">
+        <f>NOT(OR(Table1[[#This Row],[Passed?]]="yes",ISBLANK(A44)))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A3:L30 J31:L31 A31:H31 A32:L40">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="A3:L19 J32:L32 A32:H32 A33:L42 A21:L31 L18:L20">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$L3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:L30 J31:L31 A31:H31 A32:L40">
+  <conditionalFormatting sqref="A3:L19 J32:L32 A32:H32 A33:L42 A21:L31 L18:L20">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>NOT(ISBLANK($A3))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:L20">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$L20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:L20">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>NOT(ISBLANK($A3))</formula>
+      <formula>NOT(ISBLANK($A20))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correction to R vs Stata: excellent agreement achieved
for the examples in the mimix help file
</commit_message>
<xml_diff>
--- a/test/RefBasedMI testing summary.xlsx
+++ b/test/RefBasedMI testing summary.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\RefbasedMI\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2D0BF-20FD-442E-BE1F-D679654020FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAE4656-C561-49D9-8060-09022589DEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="375" yWindow="2775" windowWidth="28440" windowHeight="17535" activeTab="1" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing summary" sheetId="1" r:id="rId1"/>
+    <sheet name="R vs Stata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Testing summary'!$C$2:$K$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="119">
   <si>
     <t>Ian main testing program.R</t>
   </si>
@@ -388,12 +389,51 @@
   <si>
     <t xml:space="preserve">works perfectly, and I checked that program output matches exactly
 </t>
+  </si>
+  <si>
+    <t>estimate</t>
+  </si>
+  <si>
+    <t>std.error</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>R results</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>LMCF</t>
+  </si>
+  <si>
+    <t>J2R</t>
+  </si>
+  <si>
+    <t>CIR</t>
+  </si>
+  <si>
+    <t>MC error</t>
+  </si>
+  <si>
+    <t>Stata results</t>
+  </si>
+  <si>
+    <t>R vs Stata for the examples in the mimix help file</t>
+  </si>
+  <si>
+    <t>Z statistic, Stata - R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -510,6 +550,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,7 +1219,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1195,32 +1237,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="8" ySplit="2" topLeftCell="I12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="3"/>
-    <col min="4" max="4" width="10.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="33.21875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="42.88671875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="38.88671875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="28.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="10.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="42.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="38.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -1232,7 +1274,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:12" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1270,7 +1312,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1305,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1340,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1371,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1441,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1480,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1519,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1558,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1597,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -1636,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -1669,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
@@ -1702,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
@@ -1741,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>40</v>
       </c>
@@ -1774,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>61</v>
       </c>
@@ -1811,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>54</v>
       </c>
@@ -1846,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1869,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1892,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
@@ -1927,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="7" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>59</v>
       </c>
@@ -1964,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1987,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2014,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>100</v>
       </c>
@@ -2051,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2072,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>101</v>
       </c>
@@ -2109,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2130,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>75</v>
       </c>
@@ -2163,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2184,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>77</v>
       </c>
@@ -2215,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2238,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2263,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>79</v>
       </c>
@@ -2294,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2315,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2340,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>83</v>
       </c>
@@ -2371,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2394,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2423,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2450,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>88</v>
       </c>
@@ -2481,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2506,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>104</v>
       </c>
@@ -2554,4 +2596,212 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF80268-388E-4E90-8950-53049AF0777F}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.23854</v>
+      </c>
+      <c r="D5" s="18">
+        <v>9.8540000000000003E-2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.23854075999999999</v>
+      </c>
+      <c r="F5" s="18">
+        <v>9.8536529999999997E-2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.32844129999999999</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.1033602</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.32626279000000002</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.10383219</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2.297E-3</v>
+      </c>
+      <c r="H6" s="18">
+        <v>9.4700000000000003E-4</v>
+      </c>
+      <c r="I6" s="19">
+        <f t="shared" ref="I6:I9" si="0">(E6-C6)/(SQRT(2)*G6)</f>
+        <v>-0.67063090721927821</v>
+      </c>
+      <c r="J6" s="19">
+        <f t="shared" ref="J5:J9" si="1">(F6-D6)/(SQRT(2)*H6)</f>
+        <v>0.3524259024838885</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0.29416930000000002</v>
+      </c>
+      <c r="D7" s="18">
+        <v>9.8182350000000002E-2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.29572551000000002</v>
+      </c>
+      <c r="F7" s="18">
+        <v>9.9239270000000004E-2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>1.8779000000000001E-3</v>
+      </c>
+      <c r="H7" s="18">
+        <v>6.4070000000000002E-4</v>
+      </c>
+      <c r="I7" s="19">
+        <f t="shared" si="0"/>
+        <v>0.58597723198802842</v>
+      </c>
+      <c r="J7" s="19">
+        <f t="shared" si="1"/>
+        <v>1.166466831858417</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.22327810000000001</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.10499171</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.22448609</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0.10592255</v>
+      </c>
+      <c r="G8" s="18">
+        <v>1.9273000000000001E-3</v>
+      </c>
+      <c r="H8" s="18">
+        <v>6.7639999999999996E-4</v>
+      </c>
+      <c r="I8" s="19">
+        <f t="shared" si="0"/>
+        <v>0.44319925315494835</v>
+      </c>
+      <c r="J8" s="19">
+        <f t="shared" si="1"/>
+        <v>0.97309768805394359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.28442299999999998</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.10153821</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0.28327022000000002</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0.10248983</v>
+      </c>
+      <c r="G9" s="18">
+        <v>1.8341E-3</v>
+      </c>
+      <c r="H9" s="18">
+        <v>6.8289999999999996E-4</v>
+      </c>
+      <c r="I9" s="19">
+        <f t="shared" si="0"/>
+        <v>-0.44443517540821281</v>
+      </c>
+      <c r="J9" s="19">
+        <f t="shared" si="1"/>
+        <v>0.9853521088193623</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>